<commit_message>
Ficxed corresponding unit test
</commit_message>
<xml_diff>
--- a/tests/test-files/test_merge/expected/clean_neg_output/sheet_5.xlsx
+++ b/tests/test-files/test_merge/expected/clean_neg_output/sheet_5.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I246"/>
+  <dimension ref="A1:H246"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,7 +470,11 @@
           <t>proton_peak_index</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr"/>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>ppm</t>
+        </is>
+      </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
           <t>polymer_name</t>
@@ -478,20 +482,15 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>ppm</t>
+          <t>sample_size</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>sample_size</t>
+          <t>t_results</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>t_results</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>significance</t>
         </is>
@@ -516,15 +515,12 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0.005773502691896263</v>
+        <v>3</v>
       </c>
       <c r="G2" t="n">
-        <v>3</v>
-      </c>
-      <c r="H2" t="n">
         <v>0.002382199372125741</v>
       </c>
-      <c r="I2" t="b">
+      <c r="H2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -543,15 +539,12 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.005773502691896071</v>
+        <v>3</v>
       </c>
       <c r="G3" t="n">
-        <v>3</v>
-      </c>
-      <c r="H3" t="n">
         <v>0.02124316946578823</v>
       </c>
-      <c r="I3" t="b">
+      <c r="H3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -570,15 +563,12 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G4" t="n">
-        <v>3</v>
-      </c>
-      <c r="H4" t="n">
         <v>-0.002511188915960441</v>
       </c>
-      <c r="I4" t="b">
+      <c r="H4" t="b">
         <v>0</v>
       </c>
     </row>
@@ -597,15 +587,12 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G5" t="n">
-        <v>3</v>
-      </c>
-      <c r="H5" t="n">
         <v>-0.005803875523818162</v>
       </c>
-      <c r="I5" t="b">
+      <c r="H5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -624,15 +611,12 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G6" t="n">
-        <v>3</v>
-      </c>
-      <c r="H6" t="n">
         <v>-0.007510502921918239</v>
       </c>
-      <c r="I6" t="b">
+      <c r="H6" t="b">
         <v>0</v>
       </c>
     </row>
@@ -651,15 +635,12 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G7" t="n">
-        <v>3</v>
-      </c>
-      <c r="H7" t="n">
         <v>-0.0109040463931766</v>
       </c>
-      <c r="I7" t="b">
+      <c r="H7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -678,15 +659,12 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G8" t="n">
-        <v>3</v>
-      </c>
-      <c r="H8" t="n">
         <v>0.005230087507466235</v>
       </c>
-      <c r="I8" t="b">
+      <c r="H8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -707,15 +685,12 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>0.005773502691896263</v>
+        <v>3</v>
       </c>
       <c r="G9" t="n">
-        <v>3</v>
-      </c>
-      <c r="H9" t="n">
         <v>-0.01780638279215746</v>
       </c>
-      <c r="I9" t="b">
+      <c r="H9" t="b">
         <v>0</v>
       </c>
     </row>
@@ -734,15 +709,12 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G10" t="n">
-        <v>3</v>
-      </c>
-      <c r="H10" t="n">
         <v>-0.009054627815559876</v>
       </c>
-      <c r="I10" t="b">
+      <c r="H10" t="b">
         <v>0</v>
       </c>
     </row>
@@ -761,15 +733,12 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G11" t="n">
-        <v>3</v>
-      </c>
-      <c r="H11" t="n">
         <v>-0.008499783109670946</v>
       </c>
-      <c r="I11" t="b">
+      <c r="H11" t="b">
         <v>0</v>
       </c>
     </row>
@@ -788,15 +757,12 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G12" t="n">
-        <v>3</v>
-      </c>
-      <c r="H12" t="n">
         <v>-0.005098655263943805</v>
       </c>
-      <c r="I12" t="b">
+      <c r="H12" t="b">
         <v>0</v>
       </c>
     </row>
@@ -815,15 +781,12 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G13" t="n">
-        <v>3</v>
-      </c>
-      <c r="H13" t="n">
         <v>-0.01096350530713087</v>
       </c>
-      <c r="I13" t="b">
+      <c r="H13" t="b">
         <v>0</v>
       </c>
     </row>
@@ -842,15 +805,12 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G14" t="n">
-        <v>3</v>
-      </c>
-      <c r="H14" t="n">
         <v>-0.01156334042859705</v>
       </c>
-      <c r="I14" t="b">
+      <c r="H14" t="b">
         <v>0</v>
       </c>
     </row>
@@ -869,15 +829,12 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G15" t="n">
-        <v>3</v>
-      </c>
-      <c r="H15" t="n">
         <v>-0.0009459629668418408</v>
       </c>
-      <c r="I15" t="b">
+      <c r="H15" t="b">
         <v>0</v>
       </c>
     </row>
@@ -898,15 +855,12 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>0.005773502691896263</v>
+        <v>3</v>
       </c>
       <c r="G16" t="n">
-        <v>3</v>
-      </c>
-      <c r="H16" t="n">
         <v>0.03478047237515812</v>
       </c>
-      <c r="I16" t="b">
+      <c r="H16" t="b">
         <v>1</v>
       </c>
     </row>
@@ -925,15 +879,12 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>0.005773502691896071</v>
+        <v>3</v>
       </c>
       <c r="G17" t="n">
-        <v>3</v>
-      </c>
-      <c r="H17" t="n">
         <v>0.04399761279201861</v>
       </c>
-      <c r="I17" t="b">
+      <c r="H17" t="b">
         <v>1</v>
       </c>
     </row>
@@ -952,15 +903,12 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G18" t="n">
-        <v>3</v>
-      </c>
-      <c r="H18" t="n">
         <v>-0.001954026953442864</v>
       </c>
-      <c r="I18" t="b">
+      <c r="H18" t="b">
         <v>0</v>
       </c>
     </row>
@@ -979,15 +927,12 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G19" t="n">
-        <v>3</v>
-      </c>
-      <c r="H19" t="n">
         <v>-0.008763872772305996</v>
       </c>
-      <c r="I19" t="b">
+      <c r="H19" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1006,15 +951,12 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G20" t="n">
-        <v>3</v>
-      </c>
-      <c r="H20" t="n">
         <v>-0.00553108623272969</v>
       </c>
-      <c r="I20" t="b">
+      <c r="H20" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1033,15 +975,12 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G21" t="n">
-        <v>3</v>
-      </c>
-      <c r="H21" t="n">
         <v>-0.01419603702244092</v>
       </c>
-      <c r="I21" t="b">
+      <c r="H21" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1060,15 +999,12 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G22" t="n">
-        <v>3</v>
-      </c>
-      <c r="H22" t="n">
         <v>0.02226920360193932</v>
       </c>
-      <c r="I22" t="b">
+      <c r="H22" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1089,15 +1025,12 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>0.005773502691896263</v>
+        <v>3</v>
       </c>
       <c r="G23" t="n">
-        <v>3</v>
-      </c>
-      <c r="H23" t="n">
         <v>0.02387078275657234</v>
       </c>
-      <c r="I23" t="b">
+      <c r="H23" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1116,15 +1049,12 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>0.005773502691896071</v>
+        <v>3</v>
       </c>
       <c r="G24" t="n">
-        <v>3</v>
-      </c>
-      <c r="H24" t="n">
         <v>0.03916948730672534</v>
       </c>
-      <c r="I24" t="b">
+      <c r="H24" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1143,15 +1073,12 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G25" t="n">
-        <v>3</v>
-      </c>
-      <c r="H25" t="n">
         <v>-0.003520398616922673</v>
       </c>
-      <c r="I25" t="b">
+      <c r="H25" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1170,15 +1097,12 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G26" t="n">
-        <v>3</v>
-      </c>
-      <c r="H26" t="n">
         <v>-0.009357677942039665</v>
       </c>
-      <c r="I26" t="b">
+      <c r="H26" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1197,15 +1121,12 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G27" t="n">
-        <v>3</v>
-      </c>
-      <c r="H27" t="n">
         <v>-0.006834293301640772</v>
       </c>
-      <c r="I27" t="b">
+      <c r="H27" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1224,15 +1145,12 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G28" t="n">
-        <v>3</v>
-      </c>
-      <c r="H28" t="n">
         <v>-0.01331169245629756</v>
       </c>
-      <c r="I28" t="b">
+      <c r="H28" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1251,15 +1169,12 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G29" t="n">
-        <v>3</v>
-      </c>
-      <c r="H29" t="n">
         <v>0.03121687226281148</v>
       </c>
-      <c r="I29" t="b">
+      <c r="H29" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1280,15 +1195,12 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>0.005773502691896263</v>
+        <v>3</v>
       </c>
       <c r="G30" t="n">
-        <v>3</v>
-      </c>
-      <c r="H30" t="n">
         <v>0.01381226476294414</v>
       </c>
-      <c r="I30" t="b">
+      <c r="H30" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1307,15 +1219,12 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>0.005773502691896071</v>
+        <v>3</v>
       </c>
       <c r="G31" t="n">
-        <v>3</v>
-      </c>
-      <c r="H31" t="n">
         <v>0.01606347647788411</v>
       </c>
-      <c r="I31" t="b">
+      <c r="H31" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1334,15 +1243,12 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G32" t="n">
-        <v>3</v>
-      </c>
-      <c r="H32" t="n">
         <v>-0.005371174955311237</v>
       </c>
-      <c r="I32" t="b">
+      <c r="H32" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1361,15 +1267,12 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G33" t="n">
-        <v>3</v>
-      </c>
-      <c r="H33" t="n">
         <v>-0.007319201070260741</v>
       </c>
-      <c r="I33" t="b">
+      <c r="H33" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1388,15 +1291,12 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G34" t="n">
-        <v>3</v>
-      </c>
-      <c r="H34" t="n">
         <v>-0.01053125630949575</v>
       </c>
-      <c r="I34" t="b">
+      <c r="H34" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1415,15 +1315,12 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G35" t="n">
-        <v>3</v>
-      </c>
-      <c r="H35" t="n">
         <v>-0.01407516039978672</v>
       </c>
-      <c r="I35" t="b">
+      <c r="H35" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1442,15 +1339,12 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G36" t="n">
-        <v>3</v>
-      </c>
-      <c r="H36" t="n">
         <v>0.05123319826653616</v>
       </c>
-      <c r="I36" t="b">
+      <c r="H36" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1471,15 +1365,12 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>0.005773502691896263</v>
+        <v>3</v>
       </c>
       <c r="G37" t="n">
-        <v>3</v>
-      </c>
-      <c r="H37" t="n">
         <v>-0.02603442881979812</v>
       </c>
-      <c r="I37" t="b">
+      <c r="H37" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1498,15 +1389,12 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>0.005773502691896071</v>
+        <v>3</v>
       </c>
       <c r="G38" t="n">
-        <v>3</v>
-      </c>
-      <c r="H38" t="n">
         <v>-0.01229049279501187</v>
       </c>
-      <c r="I38" t="b">
+      <c r="H38" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1525,15 +1413,12 @@
         </is>
       </c>
       <c r="F39" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G39" t="n">
-        <v>3</v>
-      </c>
-      <c r="H39" t="n">
         <v>-0.01513299034199864</v>
       </c>
-      <c r="I39" t="b">
+      <c r="H39" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1552,15 +1437,12 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G40" t="n">
-        <v>3</v>
-      </c>
-      <c r="H40" t="n">
         <v>-0.009894414806281216</v>
       </c>
-      <c r="I40" t="b">
+      <c r="H40" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1579,15 +1461,12 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G41" t="n">
-        <v>3</v>
-      </c>
-      <c r="H41" t="n">
         <v>-0.01367217867675606</v>
       </c>
-      <c r="I41" t="b">
+      <c r="H41" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1606,15 +1485,12 @@
         </is>
       </c>
       <c r="F42" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G42" t="n">
-        <v>3</v>
-      </c>
-      <c r="H42" t="n">
         <v>-0.01727911124070991</v>
       </c>
-      <c r="I42" t="b">
+      <c r="H42" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1633,15 +1509,12 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G43" t="n">
-        <v>3</v>
-      </c>
-      <c r="H43" t="n">
         <v>0.04362534002535416</v>
       </c>
-      <c r="I43" t="b">
+      <c r="H43" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1662,15 +1535,12 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>0.005773502691896263</v>
+        <v>3</v>
       </c>
       <c r="G44" t="n">
-        <v>3</v>
-      </c>
-      <c r="H44" t="n">
         <v>0.02161023400218184</v>
       </c>
-      <c r="I44" t="b">
+      <c r="H44" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1689,15 +1559,12 @@
         </is>
       </c>
       <c r="F45" t="n">
-        <v>0.005773502691896071</v>
+        <v>3</v>
       </c>
       <c r="G45" t="n">
-        <v>3</v>
-      </c>
-      <c r="H45" t="n">
         <v>0.02603586832436706</v>
       </c>
-      <c r="I45" t="b">
+      <c r="H45" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1716,15 +1583,12 @@
         </is>
       </c>
       <c r="F46" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G46" t="n">
-        <v>3</v>
-      </c>
-      <c r="H46" t="n">
         <v>-0.001328073257524281</v>
       </c>
-      <c r="I46" t="b">
+      <c r="H46" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1743,15 +1607,12 @@
         </is>
       </c>
       <c r="F47" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G47" t="n">
-        <v>3</v>
-      </c>
-      <c r="H47" t="n">
         <v>-0.004135726995172248</v>
       </c>
-      <c r="I47" t="b">
+      <c r="H47" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1770,15 +1631,12 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G48" t="n">
-        <v>3</v>
-      </c>
-      <c r="H48" t="n">
         <v>-0.01003510855057091</v>
       </c>
-      <c r="I48" t="b">
+      <c r="H48" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1797,15 +1655,12 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G49" t="n">
-        <v>3</v>
-      </c>
-      <c r="H49" t="n">
         <v>-0.00572435673500098</v>
       </c>
-      <c r="I49" t="b">
+      <c r="H49" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1824,15 +1679,12 @@
         </is>
       </c>
       <c r="F50" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G50" t="n">
-        <v>3</v>
-      </c>
-      <c r="H50" t="n">
         <v>0.07845544423904494</v>
       </c>
-      <c r="I50" t="b">
+      <c r="H50" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1855,15 +1707,12 @@
         </is>
       </c>
       <c r="F51" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G51" t="n">
-        <v>3</v>
-      </c>
-      <c r="H51" t="n">
         <v>0.02006543019969282</v>
       </c>
-      <c r="I51" t="b">
+      <c r="H51" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1882,15 +1731,12 @@
         </is>
       </c>
       <c r="F52" t="n">
-        <v>0.009999999999999787</v>
+        <v>3</v>
       </c>
       <c r="G52" t="n">
-        <v>3</v>
-      </c>
-      <c r="H52" t="n">
         <v>0.01939711351005619</v>
       </c>
-      <c r="I52" t="b">
+      <c r="H52" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1909,15 +1755,12 @@
         </is>
       </c>
       <c r="F53" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G53" t="n">
-        <v>3</v>
-      </c>
-      <c r="H53" t="n">
         <v>0.000358745867131762</v>
       </c>
-      <c r="I53" t="b">
+      <c r="H53" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1936,15 +1779,12 @@
         </is>
       </c>
       <c r="F54" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G54" t="n">
-        <v>3</v>
-      </c>
-      <c r="H54" t="n">
         <v>-0.001330546908526516</v>
       </c>
-      <c r="I54" t="b">
+      <c r="H54" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1963,15 +1803,12 @@
         </is>
       </c>
       <c r="F55" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G55" t="n">
-        <v>3</v>
-      </c>
-      <c r="H55" t="n">
         <v>-0.001783833345459204</v>
       </c>
-      <c r="I55" t="b">
+      <c r="H55" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1990,15 +1827,12 @@
         </is>
       </c>
       <c r="F56" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G56" t="n">
-        <v>3</v>
-      </c>
-      <c r="H56" t="n">
         <v>-0.001927867932672624</v>
       </c>
-      <c r="I56" t="b">
+      <c r="H56" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2017,15 +1851,12 @@
         </is>
       </c>
       <c r="F57" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G57" t="n">
-        <v>3</v>
-      </c>
-      <c r="H57" t="n">
         <v>0.00324737257228054</v>
       </c>
-      <c r="I57" t="b">
+      <c r="H57" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2046,15 +1877,12 @@
         </is>
       </c>
       <c r="F58" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G58" t="n">
-        <v>3</v>
-      </c>
-      <c r="H58" t="n">
         <v>-0.006534026362799322</v>
       </c>
-      <c r="I58" t="b">
+      <c r="H58" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2073,15 +1901,12 @@
         </is>
       </c>
       <c r="F59" t="n">
-        <v>0.005773502691896071</v>
+        <v>3</v>
       </c>
       <c r="G59" t="n">
-        <v>3</v>
-      </c>
-      <c r="H59" t="n">
         <v>0.003115295664862954</v>
       </c>
-      <c r="I59" t="b">
+      <c r="H59" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2100,15 +1925,12 @@
         </is>
       </c>
       <c r="F60" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G60" t="n">
-        <v>3</v>
-      </c>
-      <c r="H60" t="n">
         <v>-0.0009384417944736146</v>
       </c>
-      <c r="I60" t="b">
+      <c r="H60" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2127,15 +1949,12 @@
         </is>
       </c>
       <c r="F61" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G61" t="n">
-        <v>3</v>
-      </c>
-      <c r="H61" t="n">
         <v>-0.002490784264580512</v>
       </c>
-      <c r="I61" t="b">
+      <c r="H61" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2154,15 +1973,12 @@
         </is>
       </c>
       <c r="F62" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G62" t="n">
-        <v>3</v>
-      </c>
-      <c r="H62" t="n">
         <v>-0.0006393836131531215</v>
       </c>
-      <c r="I62" t="b">
+      <c r="H62" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2181,15 +1997,12 @@
         </is>
       </c>
       <c r="F63" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G63" t="n">
-        <v>3</v>
-      </c>
-      <c r="H63" t="n">
         <v>-0.0003806029718879137</v>
       </c>
-      <c r="I63" t="b">
+      <c r="H63" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2208,15 +2021,12 @@
         </is>
       </c>
       <c r="F64" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G64" t="n">
-        <v>3</v>
-      </c>
-      <c r="H64" t="n">
         <v>0.01900987848874064</v>
       </c>
-      <c r="I64" t="b">
+      <c r="H64" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2237,15 +2047,12 @@
         </is>
       </c>
       <c r="F65" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G65" t="n">
-        <v>3</v>
-      </c>
-      <c r="H65" t="n">
         <v>0.02311333327837152</v>
       </c>
-      <c r="I65" t="b">
+      <c r="H65" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2264,15 +2071,12 @@
         </is>
       </c>
       <c r="F66" t="n">
-        <v>0.009999999999999787</v>
+        <v>3</v>
       </c>
       <c r="G66" t="n">
-        <v>3</v>
-      </c>
-      <c r="H66" t="n">
         <v>0.03147068203618431</v>
       </c>
-      <c r="I66" t="b">
+      <c r="H66" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2291,15 +2095,12 @@
         </is>
       </c>
       <c r="F67" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G67" t="n">
-        <v>3</v>
-      </c>
-      <c r="H67" t="n">
         <v>-0.00300100303514621</v>
       </c>
-      <c r="I67" t="b">
+      <c r="H67" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2318,15 +2119,12 @@
         </is>
       </c>
       <c r="F68" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G68" t="n">
-        <v>3</v>
-      </c>
-      <c r="H68" t="n">
         <v>-0.002418078916259103</v>
       </c>
-      <c r="I68" t="b">
+      <c r="H68" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2345,15 +2143,12 @@
         </is>
       </c>
       <c r="F69" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G69" t="n">
-        <v>3</v>
-      </c>
-      <c r="H69" t="n">
         <v>-0.004782909486006745</v>
       </c>
-      <c r="I69" t="b">
+      <c r="H69" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2372,15 +2167,12 @@
         </is>
       </c>
       <c r="F70" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G70" t="n">
-        <v>3</v>
-      </c>
-      <c r="H70" t="n">
         <v>-0.009023261686563467</v>
       </c>
-      <c r="I70" t="b">
+      <c r="H70" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2399,15 +2191,12 @@
         </is>
       </c>
       <c r="F71" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G71" t="n">
-        <v>3</v>
-      </c>
-      <c r="H71" t="n">
         <v>0.02052026956419701</v>
       </c>
-      <c r="I71" t="b">
+      <c r="H71" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2428,15 +2217,12 @@
         </is>
       </c>
       <c r="F72" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G72" t="n">
-        <v>3</v>
-      </c>
-      <c r="H72" t="n">
         <v>0.00550383945480688</v>
       </c>
-      <c r="I72" t="b">
+      <c r="H72" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2455,15 +2241,12 @@
         </is>
       </c>
       <c r="F73" t="n">
-        <v>0.009999999999999787</v>
+        <v>3</v>
       </c>
       <c r="G73" t="n">
-        <v>3</v>
-      </c>
-      <c r="H73" t="n">
         <v>0.01970314687643152</v>
       </c>
-      <c r="I73" t="b">
+      <c r="H73" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2482,15 +2265,12 @@
         </is>
       </c>
       <c r="F74" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G74" t="n">
-        <v>3</v>
-      </c>
-      <c r="H74" t="n">
         <v>-0.004332361771291936</v>
       </c>
-      <c r="I74" t="b">
+      <c r="H74" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2509,15 +2289,12 @@
         </is>
       </c>
       <c r="F75" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G75" t="n">
-        <v>3</v>
-      </c>
-      <c r="H75" t="n">
         <v>-0.003681275994637411</v>
       </c>
-      <c r="I75" t="b">
+      <c r="H75" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2536,15 +2313,12 @@
         </is>
       </c>
       <c r="F76" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G76" t="n">
-        <v>3</v>
-      </c>
-      <c r="H76" t="n">
         <v>0.002962405597998773</v>
       </c>
-      <c r="I76" t="b">
+      <c r="H76" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2563,15 +2337,12 @@
         </is>
       </c>
       <c r="F77" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G77" t="n">
-        <v>3</v>
-      </c>
-      <c r="H77" t="n">
         <v>-0.005439405221002617</v>
       </c>
-      <c r="I77" t="b">
+      <c r="H77" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2590,15 +2361,12 @@
         </is>
       </c>
       <c r="F78" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G78" t="n">
-        <v>3</v>
-      </c>
-      <c r="H78" t="n">
         <v>0.04395543554286815</v>
       </c>
-      <c r="I78" t="b">
+      <c r="H78" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2619,15 +2387,12 @@
         </is>
       </c>
       <c r="F79" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G79" t="n">
-        <v>3</v>
-      </c>
-      <c r="H79" t="n">
         <v>0.0002146687187379662</v>
       </c>
-      <c r="I79" t="b">
+      <c r="H79" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2646,15 +2411,12 @@
         </is>
       </c>
       <c r="F80" t="n">
-        <v>0.009999999999999787</v>
+        <v>3</v>
       </c>
       <c r="G80" t="n">
-        <v>3</v>
-      </c>
-      <c r="H80" t="n">
         <v>0.01709706230199298</v>
       </c>
-      <c r="I80" t="b">
+      <c r="H80" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2673,15 +2435,12 @@
         </is>
       </c>
       <c r="F81" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G81" t="n">
-        <v>3</v>
-      </c>
-      <c r="H81" t="n">
         <v>-0.01165463044078965</v>
       </c>
-      <c r="I81" t="b">
+      <c r="H81" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2700,15 +2459,12 @@
         </is>
       </c>
       <c r="F82" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G82" t="n">
-        <v>3</v>
-      </c>
-      <c r="H82" t="n">
         <v>-0.01112957844927979</v>
       </c>
-      <c r="I82" t="b">
+      <c r="H82" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2727,15 +2483,12 @@
         </is>
       </c>
       <c r="F83" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G83" t="n">
-        <v>3</v>
-      </c>
-      <c r="H83" t="n">
         <v>-0.008655945326692321</v>
       </c>
-      <c r="I83" t="b">
+      <c r="H83" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2754,15 +2507,12 @@
         </is>
       </c>
       <c r="F84" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G84" t="n">
-        <v>3</v>
-      </c>
-      <c r="H84" t="n">
         <v>-0.01268051103782887</v>
       </c>
-      <c r="I84" t="b">
+      <c r="H84" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2781,15 +2531,12 @@
         </is>
       </c>
       <c r="F85" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G85" t="n">
-        <v>3</v>
-      </c>
-      <c r="H85" t="n">
         <v>0.04374628394400097</v>
       </c>
-      <c r="I85" t="b">
+      <c r="H85" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2810,15 +2557,12 @@
         </is>
       </c>
       <c r="F86" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G86" t="n">
-        <v>3</v>
-      </c>
-      <c r="H86" t="n">
         <v>-0.0272445873905591</v>
       </c>
-      <c r="I86" t="b">
+      <c r="H86" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2837,15 +2581,12 @@
         </is>
       </c>
       <c r="F87" t="n">
-        <v>0.005773502691896071</v>
+        <v>3</v>
       </c>
       <c r="G87" t="n">
-        <v>3</v>
-      </c>
-      <c r="H87" t="n">
         <v>0.005161516440540158</v>
       </c>
-      <c r="I87" t="b">
+      <c r="H87" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2864,15 +2605,12 @@
         </is>
       </c>
       <c r="F88" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G88" t="n">
-        <v>3</v>
-      </c>
-      <c r="H88" t="n">
         <v>-0.01738084094001257</v>
       </c>
-      <c r="I88" t="b">
+      <c r="H88" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2891,15 +2629,12 @@
         </is>
       </c>
       <c r="F89" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G89" t="n">
-        <v>3</v>
-      </c>
-      <c r="H89" t="n">
         <v>-0.01073008041744232</v>
       </c>
-      <c r="I89" t="b">
+      <c r="H89" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2918,15 +2653,12 @@
         </is>
       </c>
       <c r="F90" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G90" t="n">
-        <v>3</v>
-      </c>
-      <c r="H90" t="n">
         <v>-0.007546643418424636</v>
       </c>
-      <c r="I90" t="b">
+      <c r="H90" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2945,15 +2677,12 @@
         </is>
       </c>
       <c r="F91" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G91" t="n">
-        <v>3</v>
-      </c>
-      <c r="H91" t="n">
         <v>-0.01354120380418164</v>
       </c>
-      <c r="I91" t="b">
+      <c r="H91" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2972,15 +2701,12 @@
         </is>
       </c>
       <c r="F92" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G92" t="n">
-        <v>3</v>
-      </c>
-      <c r="H92" t="n">
         <v>0.05323966515430117</v>
       </c>
-      <c r="I92" t="b">
+      <c r="H92" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3001,15 +2727,12 @@
         </is>
       </c>
       <c r="F93" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G93" t="n">
-        <v>3</v>
-      </c>
-      <c r="H93" t="n">
         <v>-0.01285235801943416</v>
       </c>
-      <c r="I93" t="b">
+      <c r="H93" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3028,15 +2751,12 @@
         </is>
       </c>
       <c r="F94" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G94" t="n">
-        <v>3</v>
-      </c>
-      <c r="H94" t="n">
         <v>0.006654800124440381</v>
       </c>
-      <c r="I94" t="b">
+      <c r="H94" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3055,15 +2775,12 @@
         </is>
       </c>
       <c r="F95" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G95" t="n">
-        <v>3</v>
-      </c>
-      <c r="H95" t="n">
         <v>-0.02014844242547794</v>
       </c>
-      <c r="I95" t="b">
+      <c r="H95" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3082,15 +2799,12 @@
         </is>
       </c>
       <c r="F96" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G96" t="n">
-        <v>3</v>
-      </c>
-      <c r="H96" t="n">
         <v>-0.0136281082028086</v>
       </c>
-      <c r="I96" t="b">
+      <c r="H96" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3109,15 +2823,12 @@
         </is>
       </c>
       <c r="F97" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G97" t="n">
-        <v>3</v>
-      </c>
-      <c r="H97" t="n">
         <v>-0.00856089191660734</v>
       </c>
-      <c r="I97" t="b">
+      <c r="H97" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3136,15 +2847,12 @@
         </is>
       </c>
       <c r="F98" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G98" t="n">
-        <v>3</v>
-      </c>
-      <c r="H98" t="n">
         <v>-0.01275356589830144</v>
       </c>
-      <c r="I98" t="b">
+      <c r="H98" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3163,15 +2871,12 @@
         </is>
       </c>
       <c r="F99" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G99" t="n">
-        <v>3</v>
-      </c>
-      <c r="H99" t="n">
         <v>0.07200143554527259</v>
       </c>
-      <c r="I99" t="b">
+      <c r="H99" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3194,15 +2899,12 @@
         </is>
       </c>
       <c r="F100" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G100" t="n">
-        <v>3</v>
-      </c>
-      <c r="H100" t="n">
         <v>0.004582514489731706</v>
       </c>
-      <c r="I100" t="b">
+      <c r="H100" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3221,15 +2923,12 @@
         </is>
       </c>
       <c r="F101" t="n">
-        <v>0.005773502691896071</v>
+        <v>3</v>
       </c>
       <c r="G101" t="n">
-        <v>3</v>
-      </c>
-      <c r="H101" t="n">
         <v>0.009218040661504397</v>
       </c>
-      <c r="I101" t="b">
+      <c r="H101" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3248,15 +2947,12 @@
         </is>
       </c>
       <c r="F102" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G102" t="n">
-        <v>3</v>
-      </c>
-      <c r="H102" t="n">
         <v>0.001275910958414016</v>
       </c>
-      <c r="I102" t="b">
+      <c r="H102" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3275,15 +2971,12 @@
         </is>
       </c>
       <c r="F103" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G103" t="n">
-        <v>3</v>
-      </c>
-      <c r="H103" t="n">
         <v>-9.215318753236874e-05</v>
       </c>
-      <c r="I103" t="b">
+      <c r="H103" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3302,15 +2995,12 @@
         </is>
       </c>
       <c r="F104" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G104" t="n">
-        <v>3</v>
-      </c>
-      <c r="H104" t="n">
         <v>-0.0007540673198229292</v>
       </c>
-      <c r="I104" t="b">
+      <c r="H104" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3329,15 +3019,12 @@
         </is>
       </c>
       <c r="F105" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G105" t="n">
-        <v>3</v>
-      </c>
-      <c r="H105" t="n">
         <v>-0.007312513367543372</v>
       </c>
-      <c r="I105" t="b">
+      <c r="H105" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3356,15 +3043,12 @@
         </is>
       </c>
       <c r="F106" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G106" t="n">
-        <v>3</v>
-      </c>
-      <c r="H106" t="n">
         <v>-0.02212307381852331</v>
       </c>
-      <c r="I106" t="b">
+      <c r="H106" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3385,15 +3069,12 @@
         </is>
       </c>
       <c r="F107" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G107" t="n">
-        <v>3</v>
-      </c>
-      <c r="H107" t="n">
         <v>0.002078415050087573</v>
       </c>
-      <c r="I107" t="b">
+      <c r="H107" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3412,15 +3093,12 @@
         </is>
       </c>
       <c r="F108" t="n">
-        <v>0.005773502691896263</v>
+        <v>3</v>
       </c>
       <c r="G108" t="n">
-        <v>3</v>
-      </c>
-      <c r="H108" t="n">
         <v>0.009671845026478759</v>
       </c>
-      <c r="I108" t="b">
+      <c r="H108" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3439,15 +3117,12 @@
         </is>
       </c>
       <c r="F109" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G109" t="n">
-        <v>3</v>
-      </c>
-      <c r="H109" t="n">
         <v>-0.01069622679670828</v>
       </c>
-      <c r="I109" t="b">
+      <c r="H109" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3466,15 +3141,12 @@
         </is>
       </c>
       <c r="F110" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G110" t="n">
-        <v>3</v>
-      </c>
-      <c r="H110" t="n">
         <v>-0.01073724320867977</v>
       </c>
-      <c r="I110" t="b">
+      <c r="H110" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3493,15 +3165,12 @@
         </is>
       </c>
       <c r="F111" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G111" t="n">
-        <v>3</v>
-      </c>
-      <c r="H111" t="n">
         <v>-0.01690871001190973</v>
       </c>
-      <c r="I111" t="b">
+      <c r="H111" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3520,15 +3189,12 @@
         </is>
       </c>
       <c r="F112" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G112" t="n">
-        <v>3</v>
-      </c>
-      <c r="H112" t="n">
         <v>-0.01152855963229713</v>
       </c>
-      <c r="I112" t="b">
+      <c r="H112" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3547,15 +3213,12 @@
         </is>
       </c>
       <c r="F113" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G113" t="n">
-        <v>3</v>
-      </c>
-      <c r="H113" t="n">
         <v>0.004520478542533259</v>
       </c>
-      <c r="I113" t="b">
+      <c r="H113" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3576,15 +3239,12 @@
         </is>
       </c>
       <c r="F114" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G114" t="n">
-        <v>3</v>
-      </c>
-      <c r="H114" t="n">
         <v>0.009831156625612483</v>
       </c>
-      <c r="I114" t="b">
+      <c r="H114" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3603,15 +3263,12 @@
         </is>
       </c>
       <c r="F115" t="n">
-        <v>0.005773502691896071</v>
+        <v>3</v>
       </c>
       <c r="G115" t="n">
-        <v>3</v>
-      </c>
-      <c r="H115" t="n">
         <v>0.01254758154842757</v>
       </c>
-      <c r="I115" t="b">
+      <c r="H115" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3630,15 +3287,12 @@
         </is>
       </c>
       <c r="F116" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G116" t="n">
-        <v>3</v>
-      </c>
-      <c r="H116" t="n">
         <v>-0.0107175834500701</v>
       </c>
-      <c r="I116" t="b">
+      <c r="H116" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3657,15 +3311,12 @@
         </is>
       </c>
       <c r="F117" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G117" t="n">
-        <v>3</v>
-      </c>
-      <c r="H117" t="n">
         <v>-0.00965328416129513</v>
       </c>
-      <c r="I117" t="b">
+      <c r="H117" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3684,15 +3335,12 @@
         </is>
       </c>
       <c r="F118" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G118" t="n">
-        <v>3</v>
-      </c>
-      <c r="H118" t="n">
         <v>0.003205867496994448</v>
       </c>
-      <c r="I118" t="b">
+      <c r="H118" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3711,15 +3359,12 @@
         </is>
       </c>
       <c r="F119" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G119" t="n">
-        <v>3</v>
-      </c>
-      <c r="H119" t="n">
         <v>-0.009986985630176255</v>
       </c>
-      <c r="I119" t="b">
+      <c r="H119" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3738,15 +3383,12 @@
         </is>
       </c>
       <c r="F120" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G120" t="n">
-        <v>3</v>
-      </c>
-      <c r="H120" t="n">
         <v>0.01165485912267799</v>
       </c>
-      <c r="I120" t="b">
+      <c r="H120" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3767,15 +3409,12 @@
         </is>
       </c>
       <c r="F121" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G121" t="n">
-        <v>3</v>
-      </c>
-      <c r="H121" t="n">
         <v>0.0163534787595642</v>
       </c>
-      <c r="I121" t="b">
+      <c r="H121" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3794,15 +3433,12 @@
         </is>
       </c>
       <c r="F122" t="n">
-        <v>0.005773502691896071</v>
+        <v>3</v>
       </c>
       <c r="G122" t="n">
-        <v>3</v>
-      </c>
-      <c r="H122" t="n">
         <v>0.02538295752673991</v>
       </c>
-      <c r="I122" t="b">
+      <c r="H122" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3821,15 +3457,12 @@
         </is>
       </c>
       <c r="F123" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G123" t="n">
-        <v>3</v>
-      </c>
-      <c r="H123" t="n">
         <v>-0.0118048371113879</v>
       </c>
-      <c r="I123" t="b">
+      <c r="H123" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3848,15 +3481,12 @@
         </is>
       </c>
       <c r="F124" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G124" t="n">
-        <v>3</v>
-      </c>
-      <c r="H124" t="n">
         <v>-0.01060375124574925</v>
       </c>
-      <c r="I124" t="b">
+      <c r="H124" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3875,15 +3505,12 @@
         </is>
       </c>
       <c r="F125" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G125" t="n">
-        <v>3</v>
-      </c>
-      <c r="H125" t="n">
         <v>0.006700499239935391</v>
       </c>
-      <c r="I125" t="b">
+      <c r="H125" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3902,15 +3529,12 @@
         </is>
       </c>
       <c r="F126" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G126" t="n">
-        <v>3</v>
-      </c>
-      <c r="H126" t="n">
         <v>-0.009484024610630228</v>
       </c>
-      <c r="I126" t="b">
+      <c r="H126" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3929,15 +3553,12 @@
         </is>
       </c>
       <c r="F127" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G127" t="n">
-        <v>3</v>
-      </c>
-      <c r="H127" t="n">
         <v>0.0209860079931592</v>
       </c>
-      <c r="I127" t="b">
+      <c r="H127" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3958,15 +3579,12 @@
         </is>
       </c>
       <c r="F128" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G128" t="n">
-        <v>3</v>
-      </c>
-      <c r="H128" t="n">
         <v>0.01913654474013246</v>
       </c>
-      <c r="I128" t="b">
+      <c r="H128" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3985,15 +3603,12 @@
         </is>
       </c>
       <c r="F129" t="n">
-        <v>0.005773502691896071</v>
+        <v>3</v>
       </c>
       <c r="G129" t="n">
-        <v>3</v>
-      </c>
-      <c r="H129" t="n">
         <v>0.01914992944298608</v>
       </c>
-      <c r="I129" t="b">
+      <c r="H129" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4012,15 +3627,12 @@
         </is>
       </c>
       <c r="F130" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G130" t="n">
-        <v>3</v>
-      </c>
-      <c r="H130" t="n">
         <v>-0.01274603779133954</v>
       </c>
-      <c r="I130" t="b">
+      <c r="H130" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4039,15 +3651,12 @@
         </is>
       </c>
       <c r="F131" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G131" t="n">
-        <v>3</v>
-      </c>
-      <c r="H131" t="n">
         <v>-0.01469426494149371</v>
       </c>
-      <c r="I131" t="b">
+      <c r="H131" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4066,15 +3675,12 @@
         </is>
       </c>
       <c r="F132" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G132" t="n">
-        <v>3</v>
-      </c>
-      <c r="H132" t="n">
         <v>-0.001263340732526022</v>
       </c>
-      <c r="I132" t="b">
+      <c r="H132" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4093,15 +3699,12 @@
         </is>
       </c>
       <c r="F133" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G133" t="n">
-        <v>3</v>
-      </c>
-      <c r="H133" t="n">
         <v>-0.01468341665894664</v>
       </c>
-      <c r="I133" t="b">
+      <c r="H133" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4120,15 +3723,12 @@
         </is>
       </c>
       <c r="F134" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G134" t="n">
-        <v>3</v>
-      </c>
-      <c r="H134" t="n">
         <v>0.01559870948436589</v>
       </c>
-      <c r="I134" t="b">
+      <c r="H134" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4149,15 +3749,12 @@
         </is>
       </c>
       <c r="F135" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G135" t="n">
-        <v>3</v>
-      </c>
-      <c r="H135" t="n">
         <v>0.01787032852260705</v>
       </c>
-      <c r="I135" t="b">
+      <c r="H135" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4176,15 +3773,12 @@
         </is>
       </c>
       <c r="F136" t="n">
-        <v>0.005773502691896071</v>
+        <v>3</v>
       </c>
       <c r="G136" t="n">
-        <v>3</v>
-      </c>
-      <c r="H136" t="n">
         <v>0.02875060068783774</v>
       </c>
-      <c r="I136" t="b">
+      <c r="H136" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4203,15 +3797,12 @@
         </is>
       </c>
       <c r="F137" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G137" t="n">
-        <v>3</v>
-      </c>
-      <c r="H137" t="n">
         <v>-0.01405270457275032</v>
       </c>
-      <c r="I137" t="b">
+      <c r="H137" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4230,15 +3821,12 @@
         </is>
       </c>
       <c r="F138" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G138" t="n">
-        <v>3</v>
-      </c>
-      <c r="H138" t="n">
         <v>-0.01506272163891546</v>
       </c>
-      <c r="I138" t="b">
+      <c r="H138" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4257,15 +3845,12 @@
         </is>
       </c>
       <c r="F139" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G139" t="n">
-        <v>3</v>
-      </c>
-      <c r="H139" t="n">
         <v>0.000895345983231384</v>
       </c>
-      <c r="I139" t="b">
+      <c r="H139" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4284,15 +3869,12 @@
         </is>
       </c>
       <c r="F140" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G140" t="n">
-        <v>3</v>
-      </c>
-      <c r="H140" t="n">
         <v>-0.0168302822782083</v>
       </c>
-      <c r="I140" t="b">
+      <c r="H140" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4311,15 +3893,12 @@
         </is>
       </c>
       <c r="F141" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G141" t="n">
-        <v>3</v>
-      </c>
-      <c r="H141" t="n">
         <v>0.0209383826547254</v>
       </c>
-      <c r="I141" t="b">
+      <c r="H141" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4340,15 +3919,12 @@
         </is>
       </c>
       <c r="F142" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G142" t="n">
-        <v>3</v>
-      </c>
-      <c r="H142" t="n">
         <v>0.007925851799531855</v>
       </c>
-      <c r="I142" t="b">
+      <c r="H142" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4367,15 +3943,12 @@
         </is>
       </c>
       <c r="F143" t="n">
-        <v>0.005773502691896071</v>
+        <v>3</v>
       </c>
       <c r="G143" t="n">
-        <v>3</v>
-      </c>
-      <c r="H143" t="n">
         <v>0.02660018844705355</v>
       </c>
-      <c r="I143" t="b">
+      <c r="H143" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4394,15 +3967,12 @@
         </is>
       </c>
       <c r="F144" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G144" t="n">
-        <v>3</v>
-      </c>
-      <c r="H144" t="n">
         <v>-0.01684291174309937</v>
       </c>
-      <c r="I144" t="b">
+      <c r="H144" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4421,15 +3991,12 @@
         </is>
       </c>
       <c r="F145" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G145" t="n">
-        <v>3</v>
-      </c>
-      <c r="H145" t="n">
         <v>-0.01433108922408408</v>
       </c>
-      <c r="I145" t="b">
+      <c r="H145" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4448,15 +4015,12 @@
         </is>
       </c>
       <c r="F146" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G146" t="n">
-        <v>3</v>
-      </c>
-      <c r="H146" t="n">
         <v>0.0007038098685377484</v>
       </c>
-      <c r="I146" t="b">
+      <c r="H146" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4475,15 +4039,12 @@
         </is>
       </c>
       <c r="F147" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G147" t="n">
-        <v>3</v>
-      </c>
-      <c r="H147" t="n">
         <v>-0.013434372228119</v>
       </c>
-      <c r="I147" t="b">
+      <c r="H147" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4502,15 +4063,12 @@
         </is>
       </c>
       <c r="F148" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G148" t="n">
-        <v>3</v>
-      </c>
-      <c r="H148" t="n">
         <v>0.03902609106057026</v>
       </c>
-      <c r="I148" t="b">
+      <c r="H148" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4533,15 +4091,12 @@
         </is>
       </c>
       <c r="F149" t="n">
-        <v>0.007071067811865324</v>
+        <v>2</v>
       </c>
       <c r="G149" t="n">
-        <v>2</v>
-      </c>
-      <c r="H149" t="n">
         <v>-0.4148431693903693</v>
       </c>
-      <c r="I149" t="b">
+      <c r="H149" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4560,15 +4115,12 @@
         </is>
       </c>
       <c r="F150" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G150" t="n">
-        <v>2</v>
-      </c>
-      <c r="H150" t="n">
         <v>-0.5291142680616624</v>
       </c>
-      <c r="I150" t="b">
+      <c r="H150" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4587,15 +4139,12 @@
         </is>
       </c>
       <c r="F151" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G151" t="n">
-        <v>2</v>
-      </c>
-      <c r="H151" t="n">
         <v>-0.2019540788065813</v>
       </c>
-      <c r="I151" t="b">
+      <c r="H151" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4614,15 +4163,12 @@
         </is>
       </c>
       <c r="F152" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G152" t="n">
-        <v>2</v>
-      </c>
-      <c r="H152" t="n">
         <v>-0.08611408995329273</v>
       </c>
-      <c r="I152" t="b">
+      <c r="H152" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4641,15 +4187,12 @@
         </is>
       </c>
       <c r="F153" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G153" t="n">
-        <v>2</v>
-      </c>
-      <c r="H153" t="n">
         <v>0.009551940640737836</v>
       </c>
-      <c r="I153" t="b">
+      <c r="H153" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4668,15 +4211,12 @@
         </is>
       </c>
       <c r="F154" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G154" t="n">
-        <v>2</v>
-      </c>
-      <c r="H154" t="n">
         <v>-0.008077025306483524</v>
       </c>
-      <c r="I154" t="b">
+      <c r="H154" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4695,15 +4235,12 @@
         </is>
       </c>
       <c r="F155" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G155" t="n">
-        <v>2</v>
-      </c>
-      <c r="H155" t="n">
         <v>-0.05996286037998179</v>
       </c>
-      <c r="I155" t="b">
+      <c r="H155" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4724,15 +4261,12 @@
         </is>
       </c>
       <c r="F156" t="n">
-        <v>0.007071067811865324</v>
+        <v>2</v>
       </c>
       <c r="G156" t="n">
-        <v>2</v>
-      </c>
-      <c r="H156" t="n">
         <v>-0.3968230508513133</v>
       </c>
-      <c r="I156" t="b">
+      <c r="H156" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4751,15 +4285,12 @@
         </is>
       </c>
       <c r="F157" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G157" t="n">
-        <v>2</v>
-      </c>
-      <c r="H157" t="n">
         <v>-0.4399478155281342</v>
       </c>
-      <c r="I157" t="b">
+      <c r="H157" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4778,15 +4309,12 @@
         </is>
       </c>
       <c r="F158" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G158" t="n">
-        <v>2</v>
-      </c>
-      <c r="H158" t="n">
         <v>-0.1938530098469863</v>
       </c>
-      <c r="I158" t="b">
+      <c r="H158" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4805,15 +4333,12 @@
         </is>
       </c>
       <c r="F159" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G159" t="n">
-        <v>2</v>
-      </c>
-      <c r="H159" t="n">
         <v>-0.08306656742591412</v>
       </c>
-      <c r="I159" t="b">
+      <c r="H159" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4832,15 +4357,12 @@
         </is>
       </c>
       <c r="F160" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G160" t="n">
-        <v>2</v>
-      </c>
-      <c r="H160" t="n">
         <v>0.002117980663554602</v>
       </c>
-      <c r="I160" t="b">
+      <c r="H160" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4859,15 +4381,12 @@
         </is>
       </c>
       <c r="F161" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G161" t="n">
-        <v>2</v>
-      </c>
-      <c r="H161" t="n">
         <v>-0.02571279794055454</v>
       </c>
-      <c r="I161" t="b">
+      <c r="H161" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4886,15 +4405,12 @@
         </is>
       </c>
       <c r="F162" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G162" t="n">
-        <v>2</v>
-      </c>
-      <c r="H162" t="n">
         <v>0.01877270306145576</v>
       </c>
-      <c r="I162" t="b">
+      <c r="H162" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4915,15 +4431,12 @@
         </is>
       </c>
       <c r="F163" t="n">
-        <v>0.007071067811865324</v>
+        <v>2</v>
       </c>
       <c r="G163" t="n">
-        <v>2</v>
-      </c>
-      <c r="H163" t="n">
         <v>-0.05854132956968758</v>
       </c>
-      <c r="I163" t="b">
+      <c r="H163" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4942,15 +4455,12 @@
         </is>
       </c>
       <c r="F164" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G164" t="n">
-        <v>2</v>
-      </c>
-      <c r="H164" t="n">
         <v>-0.1831034670838505</v>
       </c>
-      <c r="I164" t="b">
+      <c r="H164" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4969,15 +4479,12 @@
         </is>
       </c>
       <c r="F165" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G165" t="n">
-        <v>2</v>
-      </c>
-      <c r="H165" t="n">
         <v>-0.03433582918648939</v>
       </c>
-      <c r="I165" t="b">
+      <c r="H165" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4996,15 +4503,12 @@
         </is>
       </c>
       <c r="F166" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G166" t="n">
-        <v>2</v>
-      </c>
-      <c r="H166" t="n">
         <v>-0.05694041633324594</v>
       </c>
-      <c r="I166" t="b">
+      <c r="H166" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5023,15 +4527,12 @@
         </is>
       </c>
       <c r="F167" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G167" t="n">
-        <v>2</v>
-      </c>
-      <c r="H167" t="n">
         <v>-0.01823314669485639</v>
       </c>
-      <c r="I167" t="b">
+      <c r="H167" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5050,15 +4551,12 @@
         </is>
       </c>
       <c r="F168" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G168" t="n">
-        <v>2</v>
-      </c>
-      <c r="H168" t="n">
         <v>0.009779187849472057</v>
       </c>
-      <c r="I168" t="b">
+      <c r="H168" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5077,15 +4575,12 @@
         </is>
       </c>
       <c r="F169" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G169" t="n">
-        <v>2</v>
-      </c>
-      <c r="H169" t="n">
         <v>-0.03998236694332501</v>
       </c>
-      <c r="I169" t="b">
+      <c r="H169" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5106,15 +4601,12 @@
         </is>
       </c>
       <c r="F170" t="n">
-        <v>0.007071067811865324</v>
+        <v>2</v>
       </c>
       <c r="G170" t="n">
-        <v>2</v>
-      </c>
-      <c r="H170" t="n">
         <v>-0.7094983584820731</v>
       </c>
-      <c r="I170" t="b">
+      <c r="H170" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5133,15 +4625,12 @@
         </is>
       </c>
       <c r="F171" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G171" t="n">
-        <v>2</v>
-      </c>
-      <c r="H171" t="n">
         <v>-0.8591165404414639</v>
       </c>
-      <c r="I171" t="b">
+      <c r="H171" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5160,15 +4649,12 @@
         </is>
       </c>
       <c r="F172" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G172" t="n">
-        <v>2</v>
-      </c>
-      <c r="H172" t="n">
         <v>-0.3691147017765661</v>
       </c>
-      <c r="I172" t="b">
+      <c r="H172" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5187,15 +4673,12 @@
         </is>
       </c>
       <c r="F173" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G173" t="n">
-        <v>2</v>
-      </c>
-      <c r="H173" t="n">
         <v>-0.1720719683761938</v>
       </c>
-      <c r="I173" t="b">
+      <c r="H173" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5214,15 +4697,12 @@
         </is>
       </c>
       <c r="F174" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G174" t="n">
-        <v>2</v>
-      </c>
-      <c r="H174" t="n">
         <v>-0.02744410396703446</v>
       </c>
-      <c r="I174" t="b">
+      <c r="H174" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5241,15 +4721,12 @@
         </is>
       </c>
       <c r="F175" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G175" t="n">
-        <v>2</v>
-      </c>
-      <c r="H175" t="n">
         <v>-0.004099054431914063</v>
       </c>
-      <c r="I175" t="b">
+      <c r="H175" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5268,15 +4745,12 @@
         </is>
       </c>
       <c r="F176" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G176" t="n">
-        <v>2</v>
-      </c>
-      <c r="H176" t="n">
         <v>0.05248739570833378</v>
       </c>
-      <c r="I176" t="b">
+      <c r="H176" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5297,15 +4771,12 @@
         </is>
       </c>
       <c r="F177" t="n">
-        <v>0.007071067811865324</v>
+        <v>2</v>
       </c>
       <c r="G177" t="n">
-        <v>2</v>
-      </c>
-      <c r="H177" t="n">
         <v>-0.554908227749215</v>
       </c>
-      <c r="I177" t="b">
+      <c r="H177" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5324,15 +4795,12 @@
         </is>
       </c>
       <c r="F178" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G178" t="n">
-        <v>2</v>
-      </c>
-      <c r="H178" t="n">
         <v>-0.7646490832971151</v>
       </c>
-      <c r="I178" t="b">
+      <c r="H178" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5351,15 +4819,12 @@
         </is>
       </c>
       <c r="F179" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G179" t="n">
-        <v>2</v>
-      </c>
-      <c r="H179" t="n">
         <v>-0.2526006469591691</v>
       </c>
-      <c r="I179" t="b">
+      <c r="H179" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5378,15 +4843,12 @@
         </is>
       </c>
       <c r="F180" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G180" t="n">
-        <v>2</v>
-      </c>
-      <c r="H180" t="n">
         <v>-0.149357990021354</v>
       </c>
-      <c r="I180" t="b">
+      <c r="H180" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5405,15 +4867,12 @@
         </is>
       </c>
       <c r="F181" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G181" t="n">
-        <v>2</v>
-      </c>
-      <c r="H181" t="n">
         <v>-0.1849257039536013</v>
       </c>
-      <c r="I181" t="b">
+      <c r="H181" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5432,15 +4891,12 @@
         </is>
       </c>
       <c r="F182" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G182" t="n">
-        <v>2</v>
-      </c>
-      <c r="H182" t="n">
         <v>-0.004854479524094464</v>
       </c>
-      <c r="I182" t="b">
+      <c r="H182" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5459,15 +4915,12 @@
         </is>
       </c>
       <c r="F183" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G183" t="n">
-        <v>2</v>
-      </c>
-      <c r="H183" t="n">
         <v>0.05491727000884802</v>
       </c>
-      <c r="I183" t="b">
+      <c r="H183" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5488,15 +4941,12 @@
         </is>
       </c>
       <c r="F184" t="n">
-        <v>0.007071067811865324</v>
+        <v>2</v>
       </c>
       <c r="G184" t="n">
-        <v>2</v>
-      </c>
-      <c r="H184" t="n">
         <v>-0.6845142197694397</v>
       </c>
-      <c r="I184" t="b">
+      <c r="H184" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5515,15 +4965,12 @@
         </is>
       </c>
       <c r="F185" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G185" t="n">
-        <v>2</v>
-      </c>
-      <c r="H185" t="n">
         <v>-1.049308928212817</v>
       </c>
-      <c r="I185" t="b">
+      <c r="H185" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5542,15 +4989,12 @@
         </is>
       </c>
       <c r="F186" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G186" t="n">
-        <v>2</v>
-      </c>
-      <c r="H186" t="n">
         <v>-0.2754022406497751</v>
       </c>
-      <c r="I186" t="b">
+      <c r="H186" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5569,15 +5013,12 @@
         </is>
       </c>
       <c r="F187" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G187" t="n">
-        <v>2</v>
-      </c>
-      <c r="H187" t="n">
         <v>-0.1752438139311775</v>
       </c>
-      <c r="I187" t="b">
+      <c r="H187" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5596,15 +5037,12 @@
         </is>
       </c>
       <c r="F188" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G188" t="n">
-        <v>2</v>
-      </c>
-      <c r="H188" t="n">
         <v>-0.2770832106081426</v>
       </c>
-      <c r="I188" t="b">
+      <c r="H188" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5623,15 +5061,12 @@
         </is>
       </c>
       <c r="F189" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G189" t="n">
-        <v>2</v>
-      </c>
-      <c r="H189" t="n">
         <v>-0.0324738064532348</v>
       </c>
-      <c r="I189" t="b">
+      <c r="H189" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5650,15 +5085,12 @@
         </is>
       </c>
       <c r="F190" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G190" t="n">
-        <v>2</v>
-      </c>
-      <c r="H190" t="n">
         <v>0.05203444393297582</v>
       </c>
-      <c r="I190" t="b">
+      <c r="H190" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5679,15 +5111,12 @@
         </is>
       </c>
       <c r="F191" t="n">
-        <v>0.007071067811865324</v>
+        <v>2</v>
       </c>
       <c r="G191" t="n">
-        <v>2</v>
-      </c>
-      <c r="H191" t="n">
         <v>-0.302360648064341</v>
       </c>
-      <c r="I191" t="b">
+      <c r="H191" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5706,15 +5135,12 @@
         </is>
       </c>
       <c r="F192" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G192" t="n">
-        <v>2</v>
-      </c>
-      <c r="H192" t="n">
         <v>-0.405514539147098</v>
       </c>
-      <c r="I192" t="b">
+      <c r="H192" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5733,15 +5159,12 @@
         </is>
       </c>
       <c r="F193" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G193" t="n">
-        <v>2</v>
-      </c>
-      <c r="H193" t="n">
         <v>-0.1989504051511967</v>
       </c>
-      <c r="I193" t="b">
+      <c r="H193" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5760,15 +5183,12 @@
         </is>
       </c>
       <c r="F194" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G194" t="n">
-        <v>2</v>
-      </c>
-      <c r="H194" t="n">
         <v>-0.1451337901429939</v>
       </c>
-      <c r="I194" t="b">
+      <c r="H194" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5787,15 +5207,12 @@
         </is>
       </c>
       <c r="F195" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G195" t="n">
-        <v>2</v>
-      </c>
-      <c r="H195" t="n">
         <v>-0.1819551254863076</v>
       </c>
-      <c r="I195" t="b">
+      <c r="H195" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5814,15 +5231,12 @@
         </is>
       </c>
       <c r="F196" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G196" t="n">
-        <v>2</v>
-      </c>
-      <c r="H196" t="n">
         <v>-0.0222567410588034</v>
       </c>
-      <c r="I196" t="b">
+      <c r="H196" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5841,15 +5255,12 @@
         </is>
       </c>
       <c r="F197" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G197" t="n">
-        <v>2</v>
-      </c>
-      <c r="H197" t="n">
         <v>0.09751421357576957</v>
       </c>
-      <c r="I197" t="b">
+      <c r="H197" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5872,15 +5283,12 @@
         </is>
       </c>
       <c r="F198" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G198" t="n">
-        <v>2</v>
-      </c>
-      <c r="H198" t="n">
         <v>-0.1565228090216239</v>
       </c>
-      <c r="I198" t="b">
+      <c r="H198" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5899,15 +5307,12 @@
         </is>
       </c>
       <c r="F199" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G199" t="n">
-        <v>2</v>
-      </c>
-      <c r="H199" t="n">
         <v>-0.3079809435725689</v>
       </c>
-      <c r="I199" t="b">
+      <c r="H199" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5926,15 +5331,12 @@
         </is>
       </c>
       <c r="F200" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G200" t="n">
-        <v>2</v>
-      </c>
-      <c r="H200" t="n">
         <v>-0.09075009382622871</v>
       </c>
-      <c r="I200" t="b">
+      <c r="H200" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5953,15 +5355,12 @@
         </is>
       </c>
       <c r="F201" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G201" t="n">
-        <v>2</v>
-      </c>
-      <c r="H201" t="n">
         <v>-0.05267713455641833</v>
       </c>
-      <c r="I201" t="b">
+      <c r="H201" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5980,15 +5379,12 @@
         </is>
       </c>
       <c r="F202" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G202" t="n">
-        <v>2</v>
-      </c>
-      <c r="H202" t="n">
         <v>-0.02643005528904948</v>
       </c>
-      <c r="I202" t="b">
+      <c r="H202" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6007,15 +5403,12 @@
         </is>
       </c>
       <c r="F203" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G203" t="n">
-        <v>2</v>
-      </c>
-      <c r="H203" t="n">
         <v>0.001831998996832547</v>
       </c>
-      <c r="I203" t="b">
+      <c r="H203" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6034,15 +5427,12 @@
         </is>
       </c>
       <c r="F204" t="n">
-        <v>0.007071067811865481</v>
+        <v>2</v>
       </c>
       <c r="G204" t="n">
-        <v>2</v>
-      </c>
-      <c r="H204" t="n">
         <v>-0.01802324363346641</v>
       </c>
-      <c r="I204" t="b">
+      <c r="H204" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6063,15 +5453,12 @@
         </is>
       </c>
       <c r="F205" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G205" t="n">
-        <v>2</v>
-      </c>
-      <c r="H205" t="n">
         <v>-0.3184977747237342</v>
       </c>
-      <c r="I205" t="b">
+      <c r="H205" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6090,15 +5477,12 @@
         </is>
       </c>
       <c r="F206" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G206" t="n">
-        <v>2</v>
-      </c>
-      <c r="H206" t="n">
         <v>-0.3965998832915278</v>
       </c>
-      <c r="I206" t="b">
+      <c r="H206" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6117,15 +5501,12 @@
         </is>
       </c>
       <c r="F207" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G207" t="n">
-        <v>2</v>
-      </c>
-      <c r="H207" t="n">
         <v>-0.213580956754116</v>
       </c>
-      <c r="I207" t="b">
+      <c r="H207" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6144,15 +5525,12 @@
         </is>
       </c>
       <c r="F208" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G208" t="n">
-        <v>2</v>
-      </c>
-      <c r="H208" t="n">
         <v>-0.110210267040831</v>
       </c>
-      <c r="I208" t="b">
+      <c r="H208" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6171,15 +5549,12 @@
         </is>
       </c>
       <c r="F209" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G209" t="n">
-        <v>2</v>
-      </c>
-      <c r="H209" t="n">
         <v>-0.04491670760161967</v>
       </c>
-      <c r="I209" t="b">
+      <c r="H209" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6198,15 +5573,12 @@
         </is>
       </c>
       <c r="F210" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G210" t="n">
-        <v>2</v>
-      </c>
-      <c r="H210" t="n">
         <v>-0.004826383438795521</v>
       </c>
-      <c r="I210" t="b">
+      <c r="H210" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6225,15 +5597,12 @@
         </is>
       </c>
       <c r="F211" t="n">
-        <v>0.007071067811865481</v>
+        <v>2</v>
       </c>
       <c r="G211" t="n">
-        <v>2</v>
-      </c>
-      <c r="H211" t="n">
         <v>-0.08191543705166891</v>
       </c>
-      <c r="I211" t="b">
+      <c r="H211" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6254,15 +5623,12 @@
         </is>
       </c>
       <c r="F212" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G212" t="n">
-        <v>2</v>
-      </c>
-      <c r="H212" t="n">
         <v>-0.8007161675669907</v>
       </c>
-      <c r="I212" t="b">
+      <c r="H212" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6281,15 +5647,12 @@
         </is>
       </c>
       <c r="F213" t="n">
-        <v>0.007071067811865324</v>
+        <v>2</v>
       </c>
       <c r="G213" t="n">
-        <v>2</v>
-      </c>
-      <c r="H213" t="n">
         <v>-0.8970022103120984</v>
       </c>
-      <c r="I213" t="b">
+      <c r="H213" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6308,15 +5671,12 @@
         </is>
       </c>
       <c r="F214" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G214" t="n">
-        <v>2</v>
-      </c>
-      <c r="H214" t="n">
         <v>-0.3257176807075869</v>
       </c>
-      <c r="I214" t="b">
+      <c r="H214" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6335,15 +5695,12 @@
         </is>
       </c>
       <c r="F215" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G215" t="n">
-        <v>2</v>
-      </c>
-      <c r="H215" t="n">
         <v>-0.1577138951910782</v>
       </c>
-      <c r="I215" t="b">
+      <c r="H215" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6362,15 +5719,12 @@
         </is>
       </c>
       <c r="F216" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G216" t="n">
-        <v>2</v>
-      </c>
-      <c r="H216" t="n">
         <v>-0.04781354663192155</v>
       </c>
-      <c r="I216" t="b">
+      <c r="H216" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6389,15 +5743,12 @@
         </is>
       </c>
       <c r="F217" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G217" t="n">
-        <v>2</v>
-      </c>
-      <c r="H217" t="n">
         <v>-0.03536220748718035</v>
       </c>
-      <c r="I217" t="b">
+      <c r="H217" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6416,15 +5767,12 @@
         </is>
       </c>
       <c r="F218" t="n">
-        <v>0.007071067811865481</v>
+        <v>2</v>
       </c>
       <c r="G218" t="n">
-        <v>2</v>
-      </c>
-      <c r="H218" t="n">
         <v>-0.02399392324306859</v>
       </c>
-      <c r="I218" t="b">
+      <c r="H218" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6445,15 +5793,12 @@
         </is>
       </c>
       <c r="F219" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G219" t="n">
-        <v>2</v>
-      </c>
-      <c r="H219" t="n">
         <v>-0.2966668109188003</v>
       </c>
-      <c r="I219" t="b">
+      <c r="H219" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6472,15 +5817,12 @@
         </is>
       </c>
       <c r="F220" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G220" t="n">
-        <v>2</v>
-      </c>
-      <c r="H220" t="n">
         <v>-0.5084435484158973</v>
       </c>
-      <c r="I220" t="b">
+      <c r="H220" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6499,15 +5841,12 @@
         </is>
       </c>
       <c r="F221" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G221" t="n">
-        <v>2</v>
-      </c>
-      <c r="H221" t="n">
         <v>-0.1679529808220134</v>
       </c>
-      <c r="I221" t="b">
+      <c r="H221" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6526,15 +5865,12 @@
         </is>
       </c>
       <c r="F222" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G222" t="n">
-        <v>2</v>
-      </c>
-      <c r="H222" t="n">
         <v>-0.1637007240385742</v>
       </c>
-      <c r="I222" t="b">
+      <c r="H222" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6553,15 +5889,12 @@
         </is>
       </c>
       <c r="F223" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G223" t="n">
-        <v>2</v>
-      </c>
-      <c r="H223" t="n">
         <v>-0.2904460222382227</v>
       </c>
-      <c r="I223" t="b">
+      <c r="H223" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6580,15 +5913,12 @@
         </is>
       </c>
       <c r="F224" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G224" t="n">
-        <v>2</v>
-      </c>
-      <c r="H224" t="n">
         <v>-0.1613318812608076</v>
       </c>
-      <c r="I224" t="b">
+      <c r="H224" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6607,15 +5937,12 @@
         </is>
       </c>
       <c r="F225" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G225" t="n">
-        <v>2</v>
-      </c>
-      <c r="H225" t="n">
         <v>0.03289536412731768</v>
       </c>
-      <c r="I225" t="b">
+      <c r="H225" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6636,15 +5963,12 @@
         </is>
       </c>
       <c r="F226" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G226" t="n">
-        <v>2</v>
-      </c>
-      <c r="H226" t="n">
         <v>-0.1751910685915533</v>
       </c>
-      <c r="I226" t="b">
+      <c r="H226" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6663,15 +5987,12 @@
         </is>
       </c>
       <c r="F227" t="n">
-        <v>0.007071067811865324</v>
+        <v>2</v>
       </c>
       <c r="G227" t="n">
-        <v>2</v>
-      </c>
-      <c r="H227" t="n">
         <v>-0.1343952363865941</v>
       </c>
-      <c r="I227" t="b">
+      <c r="H227" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6690,15 +6011,12 @@
         </is>
       </c>
       <c r="F228" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G228" t="n">
-        <v>2</v>
-      </c>
-      <c r="H228" t="n">
         <v>-0.188161054807522</v>
       </c>
-      <c r="I228" t="b">
+      <c r="H228" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6717,15 +6035,12 @@
         </is>
       </c>
       <c r="F229" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G229" t="n">
-        <v>2</v>
-      </c>
-      <c r="H229" t="n">
         <v>-0.1463849314110796</v>
       </c>
-      <c r="I229" t="b">
+      <c r="H229" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6744,15 +6059,12 @@
         </is>
       </c>
       <c r="F230" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G230" t="n">
-        <v>2</v>
-      </c>
-      <c r="H230" t="n">
         <v>-0.07310588061602685</v>
       </c>
-      <c r="I230" t="b">
+      <c r="H230" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6771,15 +6083,12 @@
         </is>
       </c>
       <c r="F231" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G231" t="n">
-        <v>2</v>
-      </c>
-      <c r="H231" t="n">
         <v>-0.1591148777381244</v>
       </c>
-      <c r="I231" t="b">
+      <c r="H231" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6798,15 +6107,12 @@
         </is>
       </c>
       <c r="F232" t="n">
-        <v>0.007071067811865481</v>
+        <v>2</v>
       </c>
       <c r="G232" t="n">
-        <v>2</v>
-      </c>
-      <c r="H232" t="n">
         <v>0.007785835565799593</v>
       </c>
-      <c r="I232" t="b">
+      <c r="H232" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6827,15 +6133,12 @@
         </is>
       </c>
       <c r="F233" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G233" t="n">
-        <v>2</v>
-      </c>
-      <c r="H233" t="n">
         <v>-0.2402846100554065</v>
       </c>
-      <c r="I233" t="b">
+      <c r="H233" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6854,15 +6157,12 @@
         </is>
       </c>
       <c r="F234" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G234" t="n">
-        <v>2</v>
-      </c>
-      <c r="H234" t="n">
         <v>-0.2824447196773622</v>
       </c>
-      <c r="I234" t="b">
+      <c r="H234" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6881,15 +6181,12 @@
         </is>
       </c>
       <c r="F235" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G235" t="n">
-        <v>2</v>
-      </c>
-      <c r="H235" t="n">
         <v>-0.2086848359814376</v>
       </c>
-      <c r="I235" t="b">
+      <c r="H235" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6908,15 +6205,12 @@
         </is>
       </c>
       <c r="F236" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G236" t="n">
-        <v>2</v>
-      </c>
-      <c r="H236" t="n">
         <v>-0.1675373209755054</v>
       </c>
-      <c r="I236" t="b">
+      <c r="H236" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6935,15 +6229,12 @@
         </is>
       </c>
       <c r="F237" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G237" t="n">
-        <v>2</v>
-      </c>
-      <c r="H237" t="n">
         <v>-0.1147858504370815</v>
       </c>
-      <c r="I237" t="b">
+      <c r="H237" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6962,15 +6253,12 @@
         </is>
       </c>
       <c r="F238" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G238" t="n">
-        <v>2</v>
-      </c>
-      <c r="H238" t="n">
         <v>-0.1261965563020129</v>
       </c>
-      <c r="I238" t="b">
+      <c r="H238" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6989,15 +6277,12 @@
         </is>
       </c>
       <c r="F239" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G239" t="n">
-        <v>2</v>
-      </c>
-      <c r="H239" t="n">
         <v>0.0646725160099961</v>
       </c>
-      <c r="I239" t="b">
+      <c r="H239" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7018,15 +6303,12 @@
         </is>
       </c>
       <c r="F240" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G240" t="n">
-        <v>2</v>
-      </c>
-      <c r="H240" t="n">
         <v>-0.6483140452665134</v>
       </c>
-      <c r="I240" t="b">
+      <c r="H240" t="b">
         <v>0</v>
       </c>
     </row>
@@ -7045,15 +6327,12 @@
         </is>
       </c>
       <c r="F241" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G241" t="n">
-        <v>2</v>
-      </c>
-      <c r="H241" t="n">
         <v>-0.7043490646322143</v>
       </c>
-      <c r="I241" t="b">
+      <c r="H241" t="b">
         <v>0</v>
       </c>
     </row>
@@ -7072,15 +6351,12 @@
         </is>
       </c>
       <c r="F242" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G242" t="n">
-        <v>2</v>
-      </c>
-      <c r="H242" t="n">
         <v>-0.3628392308916158</v>
       </c>
-      <c r="I242" t="b">
+      <c r="H242" t="b">
         <v>0</v>
       </c>
     </row>
@@ -7099,15 +6375,12 @@
         </is>
       </c>
       <c r="F243" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G243" t="n">
-        <v>2</v>
-      </c>
-      <c r="H243" t="n">
         <v>-0.2297506443239269</v>
       </c>
-      <c r="I243" t="b">
+      <c r="H243" t="b">
         <v>0</v>
       </c>
     </row>
@@ -7126,15 +6399,12 @@
         </is>
       </c>
       <c r="F244" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G244" t="n">
-        <v>2</v>
-      </c>
-      <c r="H244" t="n">
         <v>-0.163289137910484</v>
       </c>
-      <c r="I244" t="b">
+      <c r="H244" t="b">
         <v>0</v>
       </c>
     </row>
@@ -7153,15 +6423,12 @@
         </is>
       </c>
       <c r="F245" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G245" t="n">
-        <v>2</v>
-      </c>
-      <c r="H245" t="n">
         <v>-0.1112829484380608</v>
       </c>
-      <c r="I245" t="b">
+      <c r="H245" t="b">
         <v>0</v>
       </c>
     </row>
@@ -7180,15 +6447,12 @@
         </is>
       </c>
       <c r="F246" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G246" t="n">
-        <v>3</v>
-      </c>
-      <c r="H246" t="n">
         <v>0.08166723345592436</v>
       </c>
-      <c r="I246" t="b">
+      <c r="H246" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>